<commit_message>
add DOC, DIC data for Toolik, Mendota, FCR DOC
</commit_message>
<xml_diff>
--- a/MacroScaleFeedbacks/Lake_Characteristics.xlsx
+++ b/MacroScaleFeedbacks/Lake_Characteristics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KJF\Desktop\R\MacrosystemsEDDIE\MacroScaleFeedbacks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618C97DC-4E30-4C80-95AA-C29CCEF2585B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C5E37F-CC38-4D7F-A670-14F99591CDFC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="726" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,9 +87,6 @@
     <t>GLEON; Lake Sunapee Protective Association</t>
   </si>
   <si>
-    <t>Data provider</t>
-  </si>
-  <si>
     <t>GLEON; Carey Lab</t>
   </si>
   <si>
@@ -106,12 +103,6 @@
   </si>
   <si>
     <t>https://www.westernvawater.org/drinking-water/water-sources-and-treatment</t>
-  </si>
-  <si>
-    <t>LTER- North Temperate Lakes</t>
-  </si>
-  <si>
-    <t>NEON Relocatable Aquatic; LTER- Arctic</t>
   </si>
   <si>
     <t>State</t>
@@ -211,6 +202,15 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>LTER- North Temperate Lakes; Hart et al. 2017</t>
+  </si>
+  <si>
+    <t>NEON Relocatable Aquatic; LTER- Arctic; Kling et al. 2000</t>
+  </si>
+  <si>
+    <t>Data providers</t>
   </si>
 </sst>
 </file>
@@ -743,28 +743,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="I1" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>5</v>
@@ -773,16 +773,16 @@
         <v>3</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>17</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -807,6 +807,9 @@
       <c r="G2" s="1">
         <v>0.12</v>
       </c>
+      <c r="H2" s="1">
+        <v>2.59</v>
+      </c>
       <c r="J2" t="s">
         <v>16</v>
       </c>
@@ -820,10 +823,10 @@
         <v>7</v>
       </c>
       <c r="N2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -848,6 +851,12 @@
       <c r="G3" s="1">
         <v>39.39</v>
       </c>
+      <c r="H3" s="1">
+        <v>4.87</v>
+      </c>
+      <c r="I3" s="1">
+        <v>45.16</v>
+      </c>
       <c r="J3" t="s">
         <v>16</v>
       </c>
@@ -861,10 +870,10 @@
         <v>6</v>
       </c>
       <c r="N3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="O3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -905,7 +914,7 @@
         <v>19</v>
       </c>
       <c r="O4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -949,10 +958,10 @@
         <v>18</v>
       </c>
       <c r="N5" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="O5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
change metadata to include DOC
</commit_message>
<xml_diff>
--- a/MacroScaleFeedbacks/Lake_Characteristics.xlsx
+++ b/MacroScaleFeedbacks/Lake_Characteristics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KJF\Desktop\R\MacrosystemsEDDIE\MacroScaleFeedbacks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C5E37F-CC38-4D7F-A670-14F99591CDFC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC471AE-6FB7-4EA0-88DA-3EA78CD7913E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="726" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -282,12 +282,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -335,7 +341,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -353,6 +359,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -810,6 +817,7 @@
       <c r="H2" s="1">
         <v>2.59</v>
       </c>
+      <c r="I2" s="9"/>
       <c r="J2" t="s">
         <v>16</v>
       </c>
@@ -898,6 +906,8 @@
       <c r="G4" s="1">
         <v>16.739999999999998</v>
       </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
       <c r="J4" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
updated Lake Characteristics spreadsheet with data on DIC & DOC for Sunapee & FCR Lowered Fsed_dic rate for Sunapee given how low those concs are!
</commit_message>
<xml_diff>
--- a/MacroScaleFeedbacks/Lake_Characteristics.xlsx
+++ b/MacroScaleFeedbacks/Lake_Characteristics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KJF\Desktop\R\MacrosystemsEDDIE\MacroScaleFeedbacks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cayelan/Dropbox/ComputerFiles/Macrosystems/Github/MacroScaleFeedbacks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC471AE-6FB7-4EA0-88DA-3EA78CD7913E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD40206-2BE5-824E-A0C5-B4881FC1C6A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="726" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3240" yWindow="9360" windowWidth="25440" windowHeight="15400" tabRatio="726" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Characteristics" sheetId="1" r:id="rId1"/>
@@ -282,18 +282,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -359,7 +353,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -725,27 +719,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.125" customWidth="1"/>
-    <col min="14" max="14" width="38.125" customWidth="1"/>
-    <col min="15" max="15" width="66.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.1640625" customWidth="1"/>
+    <col min="14" max="14" width="38.1640625" customWidth="1"/>
+    <col min="15" max="15" width="66.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -792,7 +788,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -817,7 +813,9 @@
       <c r="H2" s="1">
         <v>2.59</v>
       </c>
-      <c r="I2" s="9"/>
+      <c r="I2" s="9">
+        <v>8.3000000000000007</v>
+      </c>
       <c r="J2" t="s">
         <v>16</v>
       </c>
@@ -837,7 +835,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -884,7 +882,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -906,8 +904,12 @@
       <c r="G4" s="1">
         <v>16.739999999999998</v>
       </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
+      <c r="H4" s="9">
+        <v>2.36</v>
+      </c>
+      <c r="I4" s="9">
+        <v>2</v>
+      </c>
       <c r="J4" t="s">
         <v>6</v>
       </c>
@@ -927,7 +929,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -974,11 +976,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="O11" s="3"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O6">
+  <sortState ref="A2:O6">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>